<commit_message>
Complete the focus souce monitor.
</commit_message>
<xml_diff>
--- a/DM/maintain/monitor/Focus_Change_Log.xlsx
+++ b/DM/maintain/monitor/Focus_Change_Log.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="10420" windowWidth="19420" xWindow="-110" yWindow="-110"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="10416" windowWidth="19416" xWindow="-108" yWindow="-108"/>
   </bookViews>
   <sheets>
     <sheet name="Log" sheetId="1" state="visible" r:id="rId1"/>
@@ -15,7 +15,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt formatCode="yyyy-mm-dd" numFmtId="164"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <name val="Calibri"/>
@@ -111,7 +113,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="1" fillId="4" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -121,6 +123,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="2" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -396,31 +399,31 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane activePane="bottomRight" state="frozenSplit" topLeftCell="E3" xSplit="4" ySplit="2"/>
       <selection activeCell="D1" pane="topRight" sqref="D1"/>
       <selection activeCell="A6" pane="bottomLeft" sqref="A6"/>
-      <selection activeCell="A3" pane="bottomRight" sqref="A3:XFD12"/>
+      <selection activeCell="A3" pane="bottomRight" sqref="A3:XFD8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
   <cols>
-    <col bestFit="1" customWidth="1" max="1" min="1" style="2" width="13.453125"/>
-    <col bestFit="1" customWidth="1" max="2" min="2" style="2" width="11.6328125"/>
-    <col bestFit="1" customWidth="1" max="3" min="3" style="2" width="12.08984375"/>
-    <col bestFit="1" customWidth="1" max="4" min="4" style="2" width="14.6328125"/>
-    <col bestFit="1" customWidth="1" max="5" min="5" style="2" width="22.90625"/>
-    <col bestFit="1" customWidth="1" max="6" min="6" style="2" width="18.6328125"/>
-    <col bestFit="1" customWidth="1" max="7" min="7" style="2" width="19.08984375"/>
-    <col customWidth="1" max="8" min="8" style="2" width="19.08984375"/>
-    <col bestFit="1" customWidth="1" max="9" min="9" style="2" width="15.1796875"/>
-    <col customWidth="1" max="10" min="10" style="2" width="15.1796875"/>
-    <col bestFit="1" customWidth="1" max="11" min="11" style="2" width="16.81640625"/>
-    <col customWidth="1" max="12" min="12" style="2" width="16.81640625"/>
-    <col bestFit="1" customWidth="1" max="13" min="13" style="2" width="18.54296875"/>
-    <col customWidth="1" max="14" min="14" style="2" width="8.7265625"/>
+    <col bestFit="1" customWidth="1" max="1" min="1" style="2" width="13.44140625"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" style="2" width="11.6640625"/>
+    <col bestFit="1" customWidth="1" max="3" min="3" style="2" width="12.109375"/>
+    <col bestFit="1" customWidth="1" max="4" min="4" style="2" width="14.6640625"/>
+    <col bestFit="1" customWidth="1" max="5" min="5" style="2" width="22.88671875"/>
+    <col bestFit="1" customWidth="1" max="6" min="6" style="2" width="18.6640625"/>
+    <col bestFit="1" customWidth="1" max="7" min="7" style="2" width="19.109375"/>
+    <col customWidth="1" max="8" min="8" style="2" width="19.109375"/>
+    <col bestFit="1" customWidth="1" max="9" min="9" style="2" width="15.21875"/>
+    <col customWidth="1" max="10" min="10" style="2" width="15.21875"/>
+    <col bestFit="1" customWidth="1" max="11" min="11" style="2" width="16.77734375"/>
+    <col customWidth="1" max="12" min="12" style="2" width="16.77734375"/>
+    <col bestFit="1" customWidth="1" max="13" min="13" style="2" width="18.5546875"/>
+    <col customWidth="1" max="14" min="14" style="2" width="8.77734375"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -529,6 +532,262 @@
         <is>
           <t>NEW</t>
         </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="7" t="n">
+        <v>43693</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>,D_ADDRESS</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>AddressDetail</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>AptUnit</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>varchar</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>varchar</t>
+        </is>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>200</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>TRUE</t>
+        </is>
+      </c>
+      <c r="N3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="7" t="n">
+        <v>43693</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>,D_ADDRESS</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>AddressDetail</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>AttentionLine</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>varchar</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>varchar</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>TRUE</t>
+        </is>
+      </c>
+      <c r="N4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="7" t="n">
+        <v>43693</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>,D_ADDRESS</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>AddressDetail</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>AptUnit</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>varchar</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>varchar</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>200</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>TRUE</t>
+        </is>
+      </c>
+      <c r="N5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="7" t="n">
+        <v>43693</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>,D_ADDRESS</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>AddressDetail</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>AttentionLine</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>varchar</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>varchar</t>
+        </is>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>40</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>TRUE</t>
+        </is>
+      </c>
+      <c r="N6" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>